<commit_message>
Updating scripts according to R22 UAT 1 !
</commit_message>
<xml_diff>
--- a/Data/FundsTransferGeneral.xlsx
+++ b/Data/FundsTransferGeneral.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenium Workspace Functional Testing\Retail Ops\Data\"/>
     </mc:Choice>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>FT2236402SYQ81MM</t>
   </si>
@@ -49,12 +49,28 @@
   </si>
   <si>
     <t>FT230030XLJ94TRX</t>
+  </si>
+  <si>
+    <t>FT2316800GH03LFZ</t>
+  </si>
+  <si>
+    <t>FT231680T6161WYX</t>
+  </si>
+  <si>
+    <t>FT231680T6162257</t>
+  </si>
+  <si>
+    <t>FT2316800GH04LW6</t>
+  </si>
+  <si>
+    <t>FT2316805D7D108X</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -366,7 +382,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:A15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
@@ -424,6 +440,31 @@
         <v>9</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Committed Excel Data Updated, Sara Hasan
</commit_message>
<xml_diff>
--- a/Data/FundsTransferGeneral.xlsx
+++ b/Data/FundsTransferGeneral.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>FT2236402SYQ81MM</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>FT2316805D7D108X</t>
+  </si>
+  <si>
+    <t>FT23168119X2K9P6</t>
+  </si>
+  <si>
+    <t>FT231680RGF8G6S1</t>
   </si>
 </sst>
 </file>
@@ -382,7 +388,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A15"/>
+  <dimension ref="A1:A17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
@@ -465,6 +471,16 @@
         <v>14</v>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>